<commit_message>
Added Corridor, Door and Stairway
</commit_message>
<xml_diff>
--- a/Dokumentation/Evacuation/Example.xlsx
+++ b/Dokumentation/Evacuation/Example.xlsx
@@ -1488,9 +1488,9 @@
       <xdr:row>43</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="3622017" cy="225190"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <xdr:ext cx="4111125" cy="225190"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="Tekstfelt 6"/>
@@ -1498,8 +1498,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3886200" y="7620000"/>
-              <a:ext cx="3622017" cy="225190"/>
+              <a:off x="3886200" y="8191500"/>
+              <a:ext cx="4111125" cy="225190"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1681,7 +1681,7 @@
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>𝑚</m:t>
+                      <m:t>𝑝𝑒𝑟𝑠𝑜𝑛𝑠</m:t>
                     </m:r>
                     <m:r>
                       <a:rPr lang="da-DK" sz="1400" b="0" i="1">
@@ -1705,7 +1705,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="Tekstfelt 6"/>
@@ -1713,8 +1713,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3886200" y="7620000"/>
-              <a:ext cx="3622017" cy="225190"/>
+              <a:off x="3886200" y="8191500"/>
+              <a:ext cx="4111125" cy="225190"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1760,7 +1760,7 @@
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>∙𝑊_(𝑒,𝑐𝑜𝑟)=1,21∙2,14=2,59 𝑚/𝑠</a:t>
+                <a:t>∙𝑊_(𝑒,𝑐𝑜𝑟)=1,21∙2,14=2,59 𝑝𝑒𝑟𝑠𝑜𝑛𝑠/𝑠</a:t>
               </a:r>
               <a:endParaRPr lang="da-DK" sz="1400"/>
             </a:p>
@@ -8576,8 +8576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="M118" sqref="M118"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated html for create route elements
</commit_message>
<xml_diff>
--- a/Dokumentation/Evacuation/Example.xlsx
+++ b/Dokumentation/Evacuation/Example.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23760" windowHeight="12720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21930" windowHeight="11130"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -1489,8 +1489,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4111125" cy="225190"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="Tekstfelt 6"/>
@@ -1705,7 +1705,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="Tekstfelt 6"/>
@@ -1992,8 +1992,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5986319" cy="476990"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="Tekstfelt 8"/>
@@ -2671,7 +2671,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="Tekstfelt 8"/>
@@ -2820,8 +2820,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2536015" cy="369012"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="Tekstfelt 10"/>
@@ -2977,7 +2977,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="Tekstfelt 10"/>
@@ -3251,8 +3251,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5106078" cy="225190"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="13" name="Tekstfelt 12"/>
@@ -3442,7 +3442,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="13" name="Tekstfelt 12"/>
@@ -3515,8 +3515,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3144835" cy="225190"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="14" name="Tekstfelt 13"/>
@@ -3641,7 +3641,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="14" name="Tekstfelt 13"/>
@@ -3729,8 +3729,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4975721" cy="457561"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="16" name="Tekstfelt 15"/>
@@ -4258,7 +4258,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="16" name="Tekstfelt 15"/>
@@ -4394,8 +4394,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="6792629" cy="322781"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="17" name="Tekstfelt 16"/>
@@ -5079,7 +5079,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="17" name="Tekstfelt 16"/>
@@ -5186,8 +5186,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3519746" cy="230256"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="18" name="Tekstfelt 17"/>
@@ -5472,7 +5472,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="18" name="Tekstfelt 17"/>
@@ -5573,8 +5573,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2954976" cy="230256"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="19" name="Tekstfelt 18"/>
@@ -5859,7 +5859,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="19" name="Tekstfelt 18"/>
@@ -5960,8 +5960,8 @@
       <xdr:rowOff>134937</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4550733" cy="497572"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="Tekstfelt 7"/>
@@ -5997,6 +5997,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -6168,24 +6169,7 @@
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
-                          <m:t>1,08</m:t>
-                        </m:r>
-                        <m:r>
-                          <a:rPr kumimoji="0" lang="da-DK" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-                            <a:ln>
-                              <a:noFill/>
-                            </a:ln>
-                            <a:solidFill>
-                              <a:prstClr val="black"/>
-                            </a:solidFill>
-                            <a:effectLst/>
-                            <a:uLnTx/>
-                            <a:uFillTx/>
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="+mn-ea"/>
-                            <a:cs typeface="+mn-cs"/>
-                          </a:rPr>
-                          <m:t>±</m:t>
+                          <m:t>1,08±</m:t>
                         </m:r>
                         <m:rad>
                           <m:radPr>
@@ -6383,7 +6367,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="Tekstfelt 7"/>
@@ -6572,8 +6556,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4625497" cy="497572"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="20" name="Tekstfelt 19"/>
@@ -6609,6 +6593,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -6681,24 +6666,7 @@
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
-                          <m:t>1,08</m:t>
-                        </m:r>
-                        <m:r>
-                          <a:rPr kumimoji="0" lang="da-DK" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-                            <a:ln>
-                              <a:noFill/>
-                            </a:ln>
-                            <a:solidFill>
-                              <a:prstClr val="black"/>
-                            </a:solidFill>
-                            <a:effectLst/>
-                            <a:uLnTx/>
-                            <a:uFillTx/>
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="+mn-ea"/>
-                            <a:cs typeface="+mn-cs"/>
-                          </a:rPr>
-                          <m:t>+</m:t>
+                          <m:t>1,08+</m:t>
                         </m:r>
                         <m:rad>
                           <m:radPr>
@@ -6981,7 +6949,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="20" name="Tekstfelt 19"/>
@@ -7164,8 +7132,8 @@
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4625497" cy="497572"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="21" name="Tekstfelt 20"/>
@@ -7201,6 +7169,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -7556,7 +7525,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="21" name="Tekstfelt 20"/>
@@ -7739,8 +7708,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3542188" cy="219163"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="22" name="Tekstfelt 21"/>
@@ -7857,7 +7826,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="22" name="Tekstfelt 21"/>
@@ -7930,8 +7899,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2229072" cy="233013"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="23" name="Tekstfelt 22"/>
@@ -7974,7 +7943,6 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
-              <a:pPr/>
               <a14:m>
                 <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:sSub>
@@ -8037,7 +8005,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="23" name="Tekstfelt 22"/>
@@ -8113,8 +8081,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2881558" cy="225190"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="24" name="Tekstfelt 23"/>
@@ -8243,7 +8211,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="24" name="Tekstfelt 23"/>
@@ -8576,8 +8544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>